<commit_message>
car_type revised, wd_ratio feature added
</commit_message>
<xml_diff>
--- a/컬럼정의서.xlsx
+++ b/컬럼정의서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jomin\PycharmProjects\pythonProject\Sodescar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351DFD17-D727-4222-9B47-CA25BF7F944E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E713C86-2E15-44B5-BE23-9C3C50A9A5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8916" yWindow="564" windowWidth="17280" windowHeight="8964" xr2:uid="{B1E3BF16-E720-42C0-8C04-37A335019B0E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B1E3BF16-E720-42C0-8C04-37A335019B0E}"/>
   </bookViews>
   <sheets>
     <sheet name="socar_usage_processed.csv" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>member_age</t>
   </si>
@@ -225,10 +225,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>차종 그룹 (SUV, non_SUV)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>trip 로그상 방문한 지역들의 인구 1000명당 관광지 수 평균</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -302,6 +298,18 @@
   </si>
   <si>
     <t>상점, 위와동일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compact(경차, 소형차) / sedan(세단) / compact_SUV (소형 SUV) / SUV(소형제외 SUV) / EV(전기차) / van (승합차)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wd_ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이용시점의 평일 비율</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -309,7 +317,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +345,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -380,7 +404,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -391,6 +415,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,13 +740,13 @@
   <dimension ref="B2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="21.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.19921875" customWidth="1"/>
+    <col min="3" max="3" width="99.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.4">
@@ -832,11 +862,11 @@
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>52</v>
+      <c r="C16" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.4">
@@ -844,7 +874,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.4">
@@ -852,7 +882,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.4">
@@ -860,7 +890,7 @@
         <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -872,10 +902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877166D2-89E5-4077-A75E-58025AC56B42}">
-  <dimension ref="B2:C23"/>
+  <dimension ref="B2:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -897,7 +927,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.4">
@@ -929,135 +959,143 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>58</v>
+      <c r="B8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>71</v>
+      <c r="C24" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>